<commit_message>
feat(Employee): update template export excel
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/work_seniority.xlsx
+++ b/src/storage/app/excel-exporter/templates/work_seniority.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DS GV làm việc 3 năm trở lên" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Báo cáo thâm niên công tác" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -111,7 +111,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,12 +148,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -254,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -267,35 +261,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,7 +301,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,17 +388,17 @@
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15"/>
   </cols>
   <sheetData>
@@ -465,13 +455,13 @@
       <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -488,68 +478,68 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="10" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -572,86 +562,86 @@
       <c r="A14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
-      <c r="I17" s="14"/>
+      <c r="A17" s="13"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
-      <c r="I18" s="14"/>
+      <c r="A18" s="13"/>
+      <c r="I18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="A19" s="13"/>
+      <c r="I19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14"/>
-      <c r="I20" s="14"/>
+      <c r="A20" s="13"/>
+      <c r="I20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14"/>
-      <c r="I21" s="14"/>
+      <c r="A21" s="13"/>
+      <c r="I21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14"/>
-      <c r="I22" s="14"/>
+      <c r="A22" s="13"/>
+      <c r="I22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14"/>
-      <c r="I23" s="14"/>
+      <c r="A23" s="13"/>
+      <c r="I23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14"/>
-      <c r="I24" s="14"/>
+      <c r="A24" s="13"/>
+      <c r="I24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14"/>
-      <c r="I25" s="14"/>
+      <c r="A25" s="13"/>
+      <c r="I25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14"/>
-      <c r="I26" s="14"/>
+      <c r="A26" s="13"/>
+      <c r="I26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14"/>
-      <c r="I27" s="14"/>
+      <c r="A27" s="13"/>
+      <c r="I27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14"/>
-      <c r="I28" s="14"/>
+      <c r="A28" s="13"/>
+      <c r="I28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14"/>
-      <c r="I29" s="14"/>
+      <c r="A29" s="13"/>
+      <c r="I29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14"/>
-      <c r="I30" s="14"/>
+      <c r="A30" s="13"/>
+      <c r="I30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14"/>
-      <c r="I31" s="14"/>
+      <c r="A31" s="13"/>
+      <c r="I31" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>